<commit_message>
Exploit for case 10,14,18,22,27
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delinhoo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weikit/Desktop/cs5331-a2-exploit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFF50B2-3FFC-7544-AB55-F46C2E3878E3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CA1AC1-4E09-B94C-8107-4432E191AB2E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>Bug No.</t>
   </si>
@@ -226,13 +226,40 @@
   </si>
   <si>
     <t>S9vjABu3urWyZGU</t>
+  </si>
+  <si>
+    <t>case10.py</t>
+  </si>
+  <si>
+    <t>case14.py</t>
+  </si>
+  <si>
+    <t>EfTj7BxYg2ywfeD</t>
+  </si>
+  <si>
+    <t>A0127604L</t>
+  </si>
+  <si>
+    <t>case22.py</t>
+  </si>
+  <si>
+    <t>upcYmp7DWrwXF9k</t>
+  </si>
+  <si>
+    <t>case27.py</t>
+  </si>
+  <si>
+    <t>zwPHRtruk8T6S5s</t>
+  </si>
+  <si>
+    <t>case18.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -368,33 +395,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,11 +705,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
@@ -694,7 +721,7 @@
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -720,32 +747,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="16">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="15">
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -758,19 +785,19 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="5"/>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -780,23 +807,23 @@
       <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="5"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>3</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="5">
         <v>5</v>
       </c>
@@ -810,41 +837,41 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="5"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>2</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5">
@@ -860,13 +887,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="5">
         <v>7</v>
       </c>
@@ -880,17 +907,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>2</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="22" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5">
@@ -906,59 +933,67 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="5"/>
       <c r="F12" s="3"/>
       <c r="G12" s="7"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>2</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="E13" s="5">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="5"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>2</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="22" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="5"/>
@@ -966,29 +1001,29 @@
       <c r="G15" s="3"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="5"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="16">
         <v>2</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="23" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="5">
@@ -1004,29 +1039,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="5"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="16">
         <v>2</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="5"/>
@@ -1034,31 +1069,31 @@
       <c r="G19" s="3"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="5"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1076,7 +1111,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1094,7 +1129,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="26">
+    <row r="24" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1112,49 +1147,65 @@
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="16">
         <v>2</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="E26" s="5">
+        <v>10</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="5">
+        <v>18</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1180,29 +1231,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="16">
         <v>2</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="22" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="5"/>
@@ -1210,19 +1261,19 @@
       <c r="G30" s="3"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>26</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="5"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -1240,29 +1291,29 @@
       <c r="G32" s="3"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>28</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="16">
         <v>3</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="22" t="s">
         <v>46</v>
       </c>
       <c r="E34" s="5">
@@ -1278,31 +1329,39 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>29</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="5">
+        <v>27</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>30</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="5"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>31</v>
       </c>
@@ -1315,12 +1374,20 @@
       <c r="D37" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="E37" s="5">
+        <v>14</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>32</v>
       </c>
@@ -1338,11 +1405,11 @@
       <c r="G38" s="3"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="17" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="16"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="11">
         <f>SUM(C2:C38)</f>
         <v>32</v>
@@ -1355,6 +1422,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B29:G29"/>
@@ -1371,28 +1460,6 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Exploit for case 11,13,21,25,31 Updated case 3,14
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weikit/Desktop/cs5331-a2-exploit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CA1AC1-4E09-B94C-8107-4432E191AB2E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F56D144-66EA-2C4B-8847-69E1AB26E383}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Bug No.</t>
   </si>
@@ -253,6 +253,27 @@
   </si>
   <si>
     <t>case18.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mbyXZMR3Km6BzuH	</t>
+  </si>
+  <si>
+    <t>case11.py</t>
+  </si>
+  <si>
+    <t>case13.py</t>
+  </si>
+  <si>
+    <t>case21.py</t>
+  </si>
+  <si>
+    <t>case31.py</t>
+  </si>
+  <si>
+    <t>case25.py</t>
+  </si>
+  <si>
+    <t>MPGKgf7sHSmftp7</t>
   </si>
 </sst>
 </file>
@@ -399,9 +420,21 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -410,18 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,27 +770,27 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="18">
         <v>2</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="15">
@@ -817,10 +838,10 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="18">
         <v>3</v>
       </c>
       <c r="D6" s="17"/>
@@ -865,13 +886,13 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5">
@@ -911,13 +932,13 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="18">
         <v>2</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5">
@@ -940,22 +961,30 @@
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="4"/>
+      <c r="E12" s="5">
+        <v>31</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="18">
         <v>2</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="5">
@@ -987,13 +1016,13 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="18">
         <v>2</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="5"/>
@@ -1017,20 +1046,20 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="18">
         <v>2</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="5">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>54</v>
@@ -1046,28 +1075,44 @@
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
+      <c r="E18" s="5">
+        <v>25</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="18">
         <v>2</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="4"/>
+      <c r="E19" s="5">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1076,14 +1121,22 @@
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
+      <c r="E20" s="5">
+        <v>13</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="17"/>
@@ -1149,7 +1202,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="17"/>
@@ -1163,13 +1216,13 @@
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="18">
         <v>2</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="19" t="s">
         <v>29</v>
       </c>
       <c r="E26" s="5">
@@ -1233,7 +1286,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="17"/>
@@ -1247,13 +1300,13 @@
       <c r="A30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="18">
         <v>2</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="5"/>
@@ -1293,7 +1346,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="17"/>
@@ -1307,13 +1360,13 @@
       <c r="A34" s="1">
         <v>28</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="18">
         <v>3</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="19" t="s">
         <v>46</v>
       </c>
       <c r="E34" s="5">
@@ -1356,10 +1409,18 @@
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="4"/>
+      <c r="E36" s="5">
+        <v>11</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -1406,7 +1467,7 @@
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="18" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="17"/>
@@ -1422,28 +1483,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B29:G29"/>
@@ -1460,6 +1499,28 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Exploit for case 24
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weikit/Desktop/cs5331-a2-exploit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F56D144-66EA-2C4B-8847-69E1AB26E383}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3E9520-7BAF-EA4F-AFA3-35C826069741}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>Bug No.</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>MPGKgf7sHSmftp7</t>
+  </si>
+  <si>
+    <t>W5JAU77cnaRSNQP</t>
+  </si>
+  <si>
+    <t>case24.py</t>
   </si>
 </sst>
 </file>
@@ -384,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -419,30 +425,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,27 +777,27 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="15">
@@ -810,9 +817,9 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="5"/>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
@@ -828,7 +835,7 @@
       <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="5"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -838,13 +845,13 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>3</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="5">
         <v>5</v>
       </c>
@@ -862,9 +869,9 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -874,9 +881,9 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="5"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -886,13 +893,13 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>2</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5">
@@ -912,9 +919,9 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="5">
         <v>7</v>
       </c>
@@ -932,13 +939,13 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>2</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="23" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5">
@@ -958,9 +965,9 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="5">
         <v>31</v>
       </c>
@@ -978,13 +985,13 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>2</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="5">
@@ -1004,25 +1011,33 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="5">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <v>2</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="23" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="5"/>
@@ -1034,9 +1049,9 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="5"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1046,13 +1061,13 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="17">
         <v>2</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="24" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="5">
@@ -1072,9 +1087,9 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="5">
         <v>25</v>
       </c>
@@ -1092,13 +1107,13 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="17">
         <v>2</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="5">
@@ -1118,9 +1133,9 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="5">
         <v>13</v>
       </c>
@@ -1136,14 +1151,14 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1202,27 +1217,27 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="17">
         <v>2</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="23" t="s">
         <v>29</v>
       </c>
       <c r="E26" s="5">
@@ -1242,9 +1257,9 @@
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="5">
         <v>18</v>
       </c>
@@ -1286,27 +1301,27 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="17">
         <v>2</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="23" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="5"/>
@@ -1318,9 +1333,9 @@
       <c r="A31" s="1">
         <v>26</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="5"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1346,27 +1361,27 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>28</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="17">
         <v>3</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="23" t="s">
         <v>46</v>
       </c>
       <c r="E34" s="5">
@@ -1386,17 +1401,17 @@
       <c r="A35" s="1">
         <v>29</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="5">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>68</v>
@@ -1406,17 +1421,17 @@
       <c r="A36" s="1">
         <v>30</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="5">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>68</v>
@@ -1461,16 +1476,16 @@
       <c r="D38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="4"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="17"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="11">
         <f>SUM(C2:C38)</f>
         <v>32</v>
@@ -1479,10 +1494,35 @@
       <c r="E39" s="12"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-      <c r="H39" s="8"/>
+      <c r="H39" s="8">
+        <f>COUNTIF(H3:H37,"A*")</f>
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B29:G29"/>
@@ -1499,28 +1539,6 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Exploit for case 12 and 28
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weikit/Desktop/cs5331-a2-exploit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3E9520-7BAF-EA4F-AFA3-35C826069741}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F3BB1D-AA4F-7649-BF0A-D182ABB99811}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
   <si>
     <t>Bug No.</t>
   </si>
@@ -280,6 +280,18 @@
   </si>
   <si>
     <t>case24.py</t>
+  </si>
+  <si>
+    <t>ccCL2uX5L4kGU52</t>
+  </si>
+  <si>
+    <t>case12.py</t>
+  </si>
+  <si>
+    <t>case28.py</t>
+  </si>
+  <si>
+    <t>QG3PwQjJmsNnQrx</t>
   </si>
 </sst>
 </file>
@@ -733,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,7 +832,9 @@
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5">
+        <v>19</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
@@ -872,10 +886,18 @@
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
+      <c r="E7" s="5">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1040,10 +1062,18 @@
       <c r="D15" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
+      <c r="E15" s="5">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1052,7 +1082,9 @@
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5">
+        <v>30</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
@@ -1174,7 +1206,9 @@
       <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5">
+        <v>16</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="4"/>
@@ -1192,7 +1226,9 @@
       <c r="D23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5">
+        <v>26</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4"/>
@@ -1210,7 +1246,9 @@
       <c r="D24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5">
+        <v>9</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
@@ -1324,7 +1362,9 @@
       <c r="D30" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>17</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="4"/>
@@ -1336,7 +1376,9 @@
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5">
+        <v>20</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="4"/>
@@ -1354,7 +1396,9 @@
       <c r="D32" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5">
+        <v>23</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="4"/>
@@ -1496,7 +1540,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="8">
         <f>COUNTIF(H3:H37,"A*")</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved case06 to mixed content
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weikit/Desktop/cs5331-a2-exploit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delinhoo/5331_hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F3BB1D-AA4F-7649-BF0A-D182ABB99811}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E71BFB-5C15-CF4C-AF76-96449F702EC1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -437,11 +437,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -450,18 +464,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,27 +791,27 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="19">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="15">
@@ -859,10 +861,10 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="19">
         <v>3</v>
       </c>
       <c r="D6" s="18"/>
@@ -915,13 +917,13 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="19">
         <v>2</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5">
@@ -961,13 +963,13 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="19">
         <v>2</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5">
@@ -1007,13 +1009,13 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="19">
         <v>2</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="20" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="5">
@@ -1053,13 +1055,13 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="19">
         <v>2</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="5">
@@ -1093,13 +1095,13 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="19">
         <v>2</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="22" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="5">
@@ -1139,13 +1141,13 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="19">
         <v>2</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="22" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="5">
@@ -1183,7 +1185,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18"/>
@@ -1255,7 +1257,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="18"/>
@@ -1269,13 +1271,13 @@
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="19">
         <v>2</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="20" t="s">
         <v>29</v>
       </c>
       <c r="E26" s="5">
@@ -1325,21 +1327,15 @@
         <v>31</v>
       </c>
       <c r="E28" s="5">
-        <v>6</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="18"/>
@@ -1353,13 +1349,13 @@
       <c r="A30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="19">
         <v>2</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="20" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="5">
@@ -1405,7 +1401,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="17" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="18"/>
@@ -1419,13 +1415,13 @@
       <c r="A34" s="1">
         <v>28</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="19">
         <v>3</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="20" t="s">
         <v>46</v>
       </c>
       <c r="E34" s="5">
@@ -1520,13 +1516,21 @@
       <c r="D38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="E38" s="16">
+        <v>6</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="18"/>
@@ -1540,33 +1544,11 @@
       <c r="G39" s="7"/>
       <c r="H39" s="8">
         <f>COUNTIF(H3:H37,"A*")</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B29:G29"/>
@@ -1583,6 +1565,28 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
case 15 and case 29
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delinhoo/5331_hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E71BFB-5C15-CF4C-AF76-96449F702EC1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98D27D7-9005-2C42-A5AD-01FCEFA454C6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Bug No.</t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>QG3PwQjJmsNnQrx</t>
+  </si>
+  <si>
+    <t>case15.py</t>
+  </si>
+  <si>
+    <t>xAAy5Uvs9Stw7KZ</t>
+  </si>
+  <si>
+    <t>case29.py</t>
+  </si>
+  <si>
+    <t>42Ym92UA3uV8LVZ</t>
   </si>
 </sst>
 </file>
@@ -402,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -440,30 +452,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:G29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,27 +806,27 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="18">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="15">
@@ -831,9 +846,9 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="5">
         <v>19</v>
       </c>
@@ -851,79 +866,91 @@
       <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="17">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>3</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="5">
-        <v>5</v>
+      <c r="D6" s="19"/>
+      <c r="E6" s="17">
+        <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
+        <v>84</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="5">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5">
@@ -943,9 +970,9 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="5">
         <v>7</v>
       </c>
@@ -963,13 +990,13 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="18">
         <v>2</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="24" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5">
@@ -989,9 +1016,9 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="5">
         <v>31</v>
       </c>
@@ -1009,13 +1036,13 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>2</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="24" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="5">
@@ -1035,9 +1062,9 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="5">
         <v>24</v>
       </c>
@@ -1055,13 +1082,13 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>2</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="24" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="5">
@@ -1081,9 +1108,9 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="5">
         <v>30</v>
       </c>
@@ -1095,13 +1122,13 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="18">
         <v>2</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="25" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="5">
@@ -1121,9 +1148,9 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="5">
         <v>25</v>
       </c>
@@ -1141,13 +1168,13 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="18">
         <v>2</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="25" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="5">
@@ -1167,9 +1194,9 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="5">
         <v>13</v>
       </c>
@@ -1185,14 +1212,14 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1257,27 +1284,27 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="18">
         <v>2</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="24" t="s">
         <v>29</v>
       </c>
       <c r="E26" s="5">
@@ -1297,9 +1324,9 @@
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="5">
         <v>18</v>
       </c>
@@ -1335,27 +1362,27 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="18">
         <v>2</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="24" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="5">
@@ -1369,9 +1396,9 @@
       <c r="A31" s="1">
         <v>26</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="5">
         <v>20</v>
       </c>
@@ -1401,27 +1428,27 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>28</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="18">
         <v>3</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E34" s="5">
@@ -1441,9 +1468,9 @@
       <c r="A35" s="1">
         <v>29</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="5">
         <v>11</v>
       </c>
@@ -1461,9 +1488,9 @@
       <c r="A36" s="1">
         <v>30</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="5">
         <v>27</v>
       </c>
@@ -1530,10 +1557,10 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="18"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="11">
         <f>SUM(C2:C38)</f>
         <v>32</v>
@@ -1549,6 +1576,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B29:G29"/>
@@ -1565,28 +1614,6 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated files with .sh execution and cases
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$39</definedName>
+  </definedNames>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="108">
   <si>
     <t>Bug No.</t>
   </si>
@@ -281,39 +292,83 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>A0125471L</t>
+  </si>
+  <si>
+    <t>case17.py</t>
+  </si>
+  <si>
+    <t>case20.py</t>
+  </si>
+  <si>
+    <t>case23.py</t>
+  </si>
+  <si>
+    <t>hdls</t>
+  </si>
+  <si>
+    <t>﻿6yEJedUJsxsQY2s</t>
+  </si>
+  <si>
+    <t>﻿a53nAaEvvWSK8G3</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>raFvT7ER27j82BE</t>
+  </si>
+  <si>
+    <t>case30.py</t>
+  </si>
+  <si>
+    <t>vD7mZ27nkpJuYrp</t>
+  </si>
+  <si>
+    <t>case19.py</t>
+  </si>
+  <si>
+    <t>case32.py</t>
+  </si>
+  <si>
+    <t>﻿v6xAT3M7Ab67RDy</t>
+  </si>
+  <si>
+    <t>﻿jAGGZuEpvQ77Ekd</t>
+  </si>
+  <si>
+    <t>A0125741L</t>
+  </si>
+  <si>
+    <t>x?</t>
+  </si>
+  <si>
+    <t>working without doing anything</t>
+  </si>
+  <si>
+    <t>needs to be fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Cambria"/>
@@ -327,6 +382,18 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -343,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -411,105 +478,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -711,7 +856,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -730,7 +875,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,7 +905,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -786,7 +931,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +957,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,7 +983,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +1009,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -890,7 +1035,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -916,7 +1061,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -942,7 +1087,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -968,7 +1113,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,9 +1126,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1000,7 +1151,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1019,7 +1170,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1196,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1071,7 +1222,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,7 +1248,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1123,7 +1274,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1300,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1326,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1352,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1378,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1404,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1266,9 +1417,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1282,7 +1439,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1301,7 +1458,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1488,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1514,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1540,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1409,7 +1566,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1435,7 +1592,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1461,7 +1618,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1487,7 +1644,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1513,7 +1670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1539,7 +1696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1552,832 +1709,897 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV39"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7143" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.57812" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8672" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.2891" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.86719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.2891" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.8672" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5781" style="1" customWidth="1"/>
-    <col min="9" max="256" width="10.7344" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
+    <col min="9" max="256" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:8" ht="14.5" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
+    <row r="2" spans="1:8" ht="13.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" s="7">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" customHeight="1">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="23">
         <v>2</v>
       </c>
-      <c r="D3" t="s" s="10">
+      <c r="D3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="7">
         <v>4</v>
       </c>
-      <c r="F3" t="s" s="12">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s" s="12">
+      <c r="G3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s" s="13">
+      <c r="H3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="7">
+    <row r="4" spans="1:8" ht="17" customHeight="1">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="11">
         <v>19</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" s="7">
+      <c r="F4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" customHeight="1">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" s="7">
+      <c r="D5" s="21"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" ht="17" customHeight="1">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="10">
+      <c r="B6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="23">
         <v>3</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15">
+      <c r="D6" s="21"/>
+      <c r="E6" s="11">
         <v>5</v>
       </c>
-      <c r="F6" t="s" s="12">
+      <c r="F6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s" s="13">
+      <c r="G6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s" s="13">
+      <c r="H6" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="7">
+    <row r="7" spans="1:8" ht="17" customHeight="1">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="11">
         <v>12</v>
       </c>
-      <c r="F7" t="s" s="12">
+      <c r="F7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s" s="12">
+      <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H7" t="s" s="13">
+      <c r="H7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="7">
+    <row r="8" spans="1:8" ht="17" customHeight="1">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="14"/>
-    </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="7">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" customHeight="1">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" t="s" s="17">
+      <c r="B9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="23">
         <v>2</v>
       </c>
-      <c r="D9" t="s" s="8">
+      <c r="D9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="11">
         <v>2</v>
       </c>
-      <c r="F9" t="s" s="12">
+      <c r="F9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G9" t="s" s="12">
+      <c r="G9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H9" t="s" s="13">
+      <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="7">
+    <row r="10" spans="1:8" ht="17" customHeight="1">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15">
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="11">
         <v>7</v>
       </c>
-      <c r="F10" t="s" s="12">
+      <c r="F10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s" s="12">
+      <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H10" t="s" s="13">
+      <c r="H10" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" ht="17" customHeight="1">
-      <c r="A11" s="7">
+    <row r="11" spans="1:8" ht="17" customHeight="1">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="17">
+      <c r="B11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="23">
         <v>2</v>
       </c>
-      <c r="D11" t="s" s="8">
+      <c r="D11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="11">
         <v>8</v>
       </c>
-      <c r="F11" t="s" s="12">
+      <c r="F11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G11" t="s" s="12">
+      <c r="G11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H11" t="s" s="13">
+      <c r="H11" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" ht="17" customHeight="1">
-      <c r="A12" s="7">
+    <row r="12" spans="1:8" ht="17" customHeight="1">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="11">
         <v>31</v>
       </c>
-      <c r="F12" t="s" s="12">
+      <c r="F12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G12" t="s" s="12">
+      <c r="G12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H12" t="s" s="13">
+      <c r="H12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" ht="17" customHeight="1">
-      <c r="A13" s="7">
+    <row r="13" spans="1:8" ht="17" customHeight="1">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" t="s" s="17">
+      <c r="B13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="23">
         <v>2</v>
       </c>
-      <c r="D13" t="s" s="8">
+      <c r="D13" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="11">
         <v>22</v>
       </c>
-      <c r="F13" t="s" s="12">
+      <c r="F13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G13" t="s" s="12">
+      <c r="G13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H13" t="s" s="13">
+      <c r="H13" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" ht="17" customHeight="1">
-      <c r="A14" s="7">
+    <row r="14" spans="1:8" ht="17" customHeight="1">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="11">
         <v>24</v>
       </c>
-      <c r="F14" t="s" s="12">
+      <c r="F14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G14" t="s" s="12">
+      <c r="G14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H14" t="s" s="13">
+      <c r="H14" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" ht="17" customHeight="1">
-      <c r="A15" s="7">
+    <row r="15" spans="1:8" ht="17" customHeight="1">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" t="s" s="17">
+      <c r="B15" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="23">
         <v>2</v>
       </c>
-      <c r="D15" t="s" s="8">
+      <c r="D15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="11">
         <v>28</v>
       </c>
-      <c r="F15" t="s" s="12">
+      <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G15" t="s" s="12">
+      <c r="G15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H15" t="s" s="13">
+      <c r="H15" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" ht="17" customHeight="1">
-      <c r="A16" s="7">
+    <row r="16" spans="1:8" ht="17" customHeight="1">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="11">
         <v>30</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="14"/>
-    </row>
-    <row r="17" ht="17" customHeight="1">
-      <c r="A17" s="7">
+      <c r="F16" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" customHeight="1">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" t="s" s="17">
+      <c r="B17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="23">
         <v>2</v>
       </c>
-      <c r="D17" t="s" s="18">
+      <c r="D17" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="11">
         <v>21</v>
       </c>
-      <c r="F17" t="s" s="12">
+      <c r="F17" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G17" t="s" s="12">
+      <c r="G17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H17" t="s" s="13">
+      <c r="H17" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" ht="17" customHeight="1">
-      <c r="A18" s="7">
+    <row r="18" spans="1:9" ht="17" customHeight="1">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="11">
         <v>25</v>
       </c>
-      <c r="F18" t="s" s="12">
+      <c r="F18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G18" t="s" s="12">
+      <c r="G18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H18" t="s" s="13">
+      <c r="H18" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" ht="17" customHeight="1">
-      <c r="A19" s="7">
+    <row r="19" spans="1:9" ht="17" customHeight="1">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" t="s" s="17">
+      <c r="B19" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="23">
         <v>2</v>
       </c>
-      <c r="D19" t="s" s="18">
+      <c r="D19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="11">
         <v>3</v>
       </c>
-      <c r="F19" t="s" s="12">
+      <c r="F19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G19" t="s" s="12">
+      <c r="G19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H19" t="s" s="13">
+      <c r="H19" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" ht="17" customHeight="1">
-      <c r="A20" s="7">
+    <row r="20" spans="1:9" ht="17" customHeight="1">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="11">
         <v>13</v>
       </c>
-      <c r="F20" t="s" s="12">
+      <c r="F20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G20" t="s" s="12">
+      <c r="G20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H20" t="s" s="13">
+      <c r="H20" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" ht="17" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" t="s" s="17">
+    <row r="21" spans="1:9" ht="17" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-    </row>
-    <row r="22" ht="17" customHeight="1">
-      <c r="A22" s="7">
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" ht="17" customHeight="1">
+      <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" t="s" s="8">
+      <c r="B22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="6">
         <v>1</v>
       </c>
-      <c r="D22" t="s" s="8">
+      <c r="D22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="11">
         <v>16</v>
       </c>
-      <c r="F22" t="s" s="12">
+      <c r="F22" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="14"/>
-    </row>
-    <row r="23" ht="17" customHeight="1">
-      <c r="A23" s="7">
+      <c r="G22" s="12"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" ht="17" customHeight="1">
+      <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" t="s" s="8">
+      <c r="B23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="6">
         <v>1</v>
       </c>
-      <c r="D23" t="s" s="8">
+      <c r="D23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="11">
         <v>26</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" ht="26" customHeight="1">
-      <c r="A24" s="7">
+      <c r="F23" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="26" customHeight="1">
+      <c r="A24" s="4">
         <v>21</v>
       </c>
-      <c r="B24" t="s" s="8">
+      <c r="B24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="6">
         <v>1</v>
       </c>
-      <c r="D24" t="s" s="18">
+      <c r="D24" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="11">
         <v>9</v>
       </c>
-      <c r="F24" t="s" s="12">
+      <c r="F24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G24" t="s" s="12">
+      <c r="G24" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" ht="17" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" t="s" s="17">
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="17" customHeight="1">
+      <c r="A25" s="4"/>
+      <c r="B25" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-    </row>
-    <row r="26" ht="17" customHeight="1">
-      <c r="A26" s="7">
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" ht="17" customHeight="1">
+      <c r="A26" s="4">
         <v>22</v>
       </c>
-      <c r="B26" t="s" s="8">
+      <c r="B26" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="23">
         <v>2</v>
       </c>
-      <c r="D26" t="s" s="8">
+      <c r="D26" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="11">
         <v>10</v>
       </c>
-      <c r="F26" t="s" s="12">
+      <c r="F26" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G26" t="s" s="12">
+      <c r="G26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H26" t="s" s="13">
+      <c r="H26" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" ht="17" customHeight="1">
-      <c r="A27" s="7">
+    <row r="27" spans="1:9" ht="17" customHeight="1">
+      <c r="A27" s="4">
         <v>23</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="11">
         <v>18</v>
       </c>
-      <c r="F27" t="s" s="12">
+      <c r="F27" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G27" t="s" s="12">
+      <c r="G27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H27" t="s" s="13">
+      <c r="H27" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" ht="17" customHeight="1">
-      <c r="A28" s="7">
+    <row r="28" spans="1:9" ht="17" customHeight="1">
+      <c r="A28" s="4">
         <v>24</v>
       </c>
-      <c r="B28" t="s" s="8">
+      <c r="B28" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="D28" t="s" s="8">
+      <c r="D28" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="11">
         <v>6</v>
       </c>
-      <c r="F28" t="s" s="12">
+      <c r="F28" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G28" t="s" s="12">
+      <c r="G28" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H28" t="s" s="13">
+      <c r="H28" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" ht="17" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" t="s" s="17">
+    <row r="29" spans="1:9" ht="17" customHeight="1">
+      <c r="A29" s="4"/>
+      <c r="B29" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" ht="17" customHeight="1">
-      <c r="A30" s="7">
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:9" ht="17" customHeight="1">
+      <c r="A30" s="4">
         <v>25</v>
       </c>
-      <c r="B30" t="s" s="8">
+      <c r="B30" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="23">
         <v>2</v>
       </c>
-      <c r="D30" t="s" s="8">
+      <c r="D30" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="11">
         <v>17</v>
       </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" ht="17" customHeight="1">
-      <c r="A31" s="7">
+      <c r="F30" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" customHeight="1">
+      <c r="A31" s="4">
         <v>26</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="15">
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="11">
         <v>20</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="14"/>
-    </row>
-    <row r="32" ht="17" customHeight="1">
-      <c r="A32" s="7">
+      <c r="F31" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17" customHeight="1">
+      <c r="A32" s="4">
         <v>27</v>
       </c>
-      <c r="B32" t="s" s="8">
+      <c r="B32" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="6">
         <v>1</v>
       </c>
-      <c r="D32" t="s" s="8">
+      <c r="D32" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="11">
         <v>23</v>
       </c>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" ht="17" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" t="s" s="17">
+      <c r="F32" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="17" customHeight="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-    </row>
-    <row r="34" ht="17" customHeight="1">
-      <c r="A34" s="7">
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="1:9" ht="17" customHeight="1">
+      <c r="A34" s="4">
         <v>28</v>
       </c>
-      <c r="B34" t="s" s="8">
+      <c r="B34" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="23">
         <v>3</v>
       </c>
-      <c r="D34" t="s" s="8">
+      <c r="D34" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="11">
         <v>1</v>
       </c>
-      <c r="F34" t="s" s="12">
+      <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G34" t="s" s="12">
+      <c r="G34" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H34" t="s" s="13">
+      <c r="H34" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" ht="17" customHeight="1">
-      <c r="A35" s="7">
+    <row r="35" spans="1:9" ht="17" customHeight="1">
+      <c r="A35" s="4">
         <v>29</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="15">
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="11">
         <v>11</v>
       </c>
-      <c r="F35" t="s" s="12">
+      <c r="F35" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G35" t="s" s="12">
+      <c r="G35" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H35" t="s" s="13">
+      <c r="H35" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="17" customHeight="1">
-      <c r="A36" s="7">
+    <row r="36" spans="1:9" ht="17" customHeight="1">
+      <c r="A36" s="4">
         <v>30</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="15">
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="11">
         <v>27</v>
       </c>
-      <c r="F36" t="s" s="12">
+      <c r="F36" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G36" t="s" s="12">
+      <c r="G36" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H36" t="s" s="13">
+      <c r="H36" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" ht="17" customHeight="1">
-      <c r="A37" s="7">
+    <row r="37" spans="1:9" ht="17" customHeight="1">
+      <c r="A37" s="4">
         <v>31</v>
       </c>
-      <c r="B37" t="s" s="8">
+      <c r="B37" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="6">
         <v>1</v>
       </c>
-      <c r="D37" t="s" s="8">
+      <c r="D37" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="11">
         <v>14</v>
       </c>
-      <c r="F37" t="s" s="12">
+      <c r="F37" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G37" t="s" s="12">
+      <c r="G37" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H37" t="s" s="13">
+      <c r="H37" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="17" customHeight="1">
-      <c r="A38" s="7">
+    <row r="38" spans="1:9" ht="17" customHeight="1">
+      <c r="A38" s="4">
         <v>32</v>
       </c>
-      <c r="B38" t="s" s="17">
+      <c r="B38" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" t="s" s="8">
+      <c r="D38" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-    </row>
-    <row r="39" ht="17" customHeight="1">
-      <c r="A39" t="s" s="19">
+      <c r="E38" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="17" customHeight="1">
+      <c r="A39" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="20">
+      <c r="B39" s="21"/>
+      <c r="C39" s="15">
         <f>SUM(C2:C38)</f>
         <v>32</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="14">
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="10">
         <f>COUNTIF(H3:H37,"A*")</f>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H39"/>
   <mergeCells count="38">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="D26:D27"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="B25:G25"/>
@@ -2394,26 +2616,22 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="B34:B36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B29:G29"/>
     <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding case 15 and 29
</commit_message>
<xml_diff>
--- a/BUG_REPORT.xlsx
+++ b/BUG_REPORT.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delinhoo/5331_hw2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC329FF7-48E5-B249-B31A-B9A61C7021BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16420"/>
+    <workbookView xWindow="1020" yWindow="480" windowWidth="18040" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$39</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
   <si>
     <t>Bug No.</t>
   </si>
@@ -342,19 +348,25 @@
     <t>A0125741L</t>
   </si>
   <si>
-    <t>x?</t>
-  </si>
-  <si>
     <t>working without doing anything</t>
   </si>
   <si>
-    <t>needs to be fixed</t>
+    <t>case15.py</t>
+  </si>
+  <si>
+    <t>xAAy5Uvs9Stw7KZ</t>
+  </si>
+  <si>
+    <t>case29.py</t>
+  </si>
+  <si>
+    <t>42Ym92UA3uV8LVZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -537,20 +549,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -563,12 +581,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -650,6 +662,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1727,14 +1747,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="1" customWidth="1"/>
@@ -1747,7 +1767,7 @@
     <col min="9" max="256" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" customHeight="1">
+    <row r="1" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1773,29 +1793,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1">
+    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-    </row>
-    <row r="3" spans="1:8" ht="17" customHeight="1">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
         <v>2</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="22" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="7">
@@ -1811,7 +1831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17" customHeight="1">
+    <row r="4" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1831,7 +1851,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" customHeight="1">
+    <row r="5" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1842,36 +1862,44 @@
         <v>1</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" ht="17" customHeight="1">
+      <c r="E5" s="11">
+        <v>5</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="24">
         <v>3</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="11">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1879,41 +1907,45 @@
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="11">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" customHeight="1">
+        <v>107</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="E8" s="11">
+        <v>29</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>109</v>
+      </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" ht="17" customHeight="1">
+    <row r="9" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="24">
         <v>2</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="11">
@@ -1929,7 +1961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" customHeight="1">
+    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1949,17 +1981,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" customHeight="1">
+    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="24">
         <v>2</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="23" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="11">
@@ -1975,7 +2007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" customHeight="1">
+    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1995,17 +2027,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" customHeight="1">
+    <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="24">
         <v>2</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="23" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="11">
@@ -2021,7 +2053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17" customHeight="1">
+    <row r="14" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -2041,17 +2073,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17" customHeight="1">
+    <row r="15" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="24">
         <v>2</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="11">
@@ -2067,7 +2099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" customHeight="1">
+    <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -2087,17 +2119,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17" customHeight="1">
+    <row r="17" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="24">
         <v>2</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="25" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="11">
@@ -2113,7 +2145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17" customHeight="1">
+    <row r="18" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -2133,17 +2165,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17" customHeight="1">
+    <row r="19" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="24">
         <v>2</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E19" s="11">
@@ -2159,7 +2191,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="17" customHeight="1">
+    <row r="20" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -2179,9 +2211,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17" customHeight="1">
+    <row r="21" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="21"/>
@@ -2191,7 +2223,7 @@
       <c r="G21" s="21"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="17" customHeight="1">
+    <row r="22" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -2213,7 +2245,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="17" customHeight="1">
+    <row r="23" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>20</v>
       </c>
@@ -2236,10 +2268,10 @@
         <v>103</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="26" customHeight="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -2263,9 +2295,9 @@
       </c>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="17" customHeight="1">
+    <row r="25" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="21"/>
@@ -2275,17 +2307,17 @@
       <c r="G25" s="21"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="17" customHeight="1">
+    <row r="26" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>22</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="24">
         <v>2</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="23" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="11">
@@ -2301,7 +2333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17" customHeight="1">
+    <row r="27" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>23</v>
       </c>
@@ -2321,7 +2353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17" customHeight="1">
+    <row r="28" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>24</v>
       </c>
@@ -2334,22 +2366,22 @@
       <c r="D28" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="11">
-        <v>6</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="17" customHeight="1">
+      <c r="E28" s="19">
+        <v>32</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="20" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="21"/>
@@ -2359,17 +2391,17 @@
       <c r="G29" s="21"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="17" customHeight="1">
+    <row r="30" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>25</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="24">
         <v>2</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="23" t="s">
         <v>70</v>
       </c>
       <c r="E30" s="11">
@@ -2385,7 +2417,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17" customHeight="1">
+    <row r="31" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>26</v>
       </c>
@@ -2398,14 +2430,14 @@
       <c r="F31" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="17" t="s">
         <v>94</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17" customHeight="1">
+    <row r="32" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>27</v>
       </c>
@@ -2431,9 +2463,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17" customHeight="1">
+    <row r="33" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="20" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="21"/>
@@ -2442,17 +2474,17 @@
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="34" spans="1:9" ht="17" customHeight="1">
+    <row r="34" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>28</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="24">
         <v>3</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="23" t="s">
         <v>75</v>
       </c>
       <c r="E34" s="11">
@@ -2468,7 +2500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17" customHeight="1">
+    <row r="35" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>29</v>
       </c>
@@ -2488,7 +2520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="17" customHeight="1">
+    <row r="36" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>30</v>
       </c>
@@ -2508,7 +2540,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="17" customHeight="1">
+    <row r="37" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>31</v>
       </c>
@@ -2534,7 +2566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="17" customHeight="1">
+    <row r="38" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>32</v>
       </c>
@@ -2547,24 +2579,22 @@
       <c r="D38" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I38" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="17" customHeight="1">
-      <c r="A39" s="27" t="s">
+      <c r="E38" s="11">
+        <v>6</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="21"/>
@@ -2582,8 +2612,30 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H39"/>
+  <autoFilter ref="A1:H39" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="38">
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B34:B36"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="B30:B31"/>
@@ -2600,28 +2652,6 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>